<commit_message>
- updated export templates
</commit_message>
<xml_diff>
--- a/jems-ui/e2e/cypress/fixtures/project/application-form/project-budget/TB-383-export.xlsx
+++ b/jems-ui/e2e/cypress/fixtures/project/application-form/project-budget/TB-383-export.xlsx
@@ -6,8 +6,8 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Project_budget_00162_1080p band" r:id="rId3" sheetId="1"/>
-    <sheet name="Partner_budget_00162_1080p band" r:id="rId4" sheetId="2"/>
+    <sheet name="Project_budget_00085_digital in" r:id="rId3" sheetId="1"/>
+    <sheet name="Partner_budget_00085_digital in" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
@@ -417,41 +417,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="51.56640625" customWidth="true"/>
-    <col min="2" max="2" width="6.58984375" customWidth="true"/>
-    <col min="3" max="3" width="24.31640625" customWidth="true"/>
-    <col min="4" max="4" width="41.75" customWidth="true"/>
-    <col min="5" max="5" width="32.7890625" customWidth="true"/>
-    <col min="6" max="6" width="8.1796875" customWidth="true"/>
-    <col min="7" max="7" width="15.2265625" customWidth="true"/>
-    <col min="8" max="8" width="17.83984375" customWidth="true"/>
-    <col min="9" max="9" width="14.453125" customWidth="true"/>
-    <col min="10" max="10" width="14.5859375" customWidth="true"/>
-    <col min="11" max="11" width="34.51171875" customWidth="true"/>
-    <col min="12" max="12" width="37.4375" customWidth="true"/>
-    <col min="13" max="13" width="31.26171875" customWidth="true"/>
-    <col min="14" max="14" width="33.01171875" customWidth="true"/>
-    <col min="15" max="15" width="34.671875" customWidth="true"/>
-    <col min="16" max="16" width="34.8046875" customWidth="true"/>
-    <col min="17" max="17" width="34.4609375" customWidth="true"/>
-    <col min="18" max="18" width="37.875" customWidth="true"/>
-    <col min="19" max="19" width="38.0078125" customWidth="true"/>
-    <col min="20" max="20" width="19.1875" customWidth="true"/>
-    <col min="21" max="21" width="24.4140625" customWidth="true"/>
-    <col min="22" max="22" width="20.234375" customWidth="true"/>
-    <col min="23" max="23" width="29.0234375" customWidth="true"/>
-    <col min="24" max="24" width="32.4375" customWidth="true"/>
-    <col min="25" max="25" width="32.5703125" customWidth="true"/>
-    <col min="26" max="26" width="11.29296875" customWidth="true"/>
-    <col min="27" max="27" width="10.30078125" customWidth="true"/>
-    <col min="28" max="28" width="44.26953125" customWidth="true"/>
-    <col min="29" max="29" width="19.29296875" customWidth="true"/>
+    <col min="1" max="1" width="51.609375" customWidth="true"/>
+    <col min="2" max="2" width="6.8828125" customWidth="true"/>
+    <col min="3" max="3" width="24.93359375" customWidth="true"/>
+    <col min="4" max="4" width="43.20703125" customWidth="true"/>
+    <col min="5" max="5" width="33.82421875" customWidth="true"/>
+    <col min="6" max="6" width="8.32421875" customWidth="true"/>
+    <col min="7" max="7" width="15.74609375" customWidth="true"/>
+    <col min="8" max="8" width="18.56640625" customWidth="true"/>
+    <col min="9" max="9" width="15.06640625" customWidth="true"/>
+    <col min="10" max="10" width="15.10546875" customWidth="true"/>
+    <col min="11" max="11" width="35.64453125" customWidth="true"/>
+    <col min="12" max="12" width="38.75390625" customWidth="true"/>
+    <col min="13" max="13" width="32.1484375" customWidth="true"/>
+    <col min="14" max="14" width="34.015625" customWidth="true"/>
+    <col min="15" max="15" width="35.859375" customWidth="true"/>
+    <col min="16" max="16" width="35.89453125" customWidth="true"/>
+    <col min="17" max="17" width="35.98828125" customWidth="true"/>
+    <col min="18" max="18" width="39.69921875" customWidth="true"/>
+    <col min="19" max="19" width="39.734375" customWidth="true"/>
+    <col min="20" max="20" width="19.43359375" customWidth="true"/>
+    <col min="21" max="21" width="24.71484375" customWidth="true"/>
+    <col min="22" max="22" width="20.7578125" customWidth="true"/>
+    <col min="23" max="23" width="29.65234375" customWidth="true"/>
+    <col min="24" max="24" width="33.36328125" customWidth="true"/>
+    <col min="25" max="25" width="33.3984375" customWidth="true"/>
+    <col min="26" max="26" width="11.58984375" customWidth="true"/>
+    <col min="27" max="27" width="10.66015625" customWidth="true"/>
+    <col min="28" max="28" width="45.81640625" customWidth="true"/>
+    <col min="29" max="29" width="19.921875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>00162 - 1080p bandwidth - V1.0 - 2022/12/05 - 15:08:40</t>
+          <t>00085 - digital interface - V1.0 - 2023/06/20 - 11:27:54</t>
         </is>
       </c>
     </row>
@@ -1316,37 +1316,37 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="51.56640625" customWidth="true"/>
-    <col min="2" max="2" width="6.58984375" customWidth="true"/>
-    <col min="3" max="3" width="24.31640625" customWidth="true"/>
-    <col min="4" max="4" width="41.75" customWidth="true"/>
-    <col min="5" max="5" width="32.7890625" customWidth="true"/>
-    <col min="6" max="6" width="8.1796875" customWidth="true"/>
-    <col min="7" max="7" width="7.5625" customWidth="true"/>
-    <col min="8" max="8" width="7.5625" customWidth="true"/>
-    <col min="9" max="9" width="25.3984375" customWidth="true"/>
-    <col min="10" max="10" width="41.625" customWidth="true"/>
-    <col min="11" max="11" width="41.05078125" customWidth="true"/>
-    <col min="12" max="12" width="17.49609375" customWidth="true"/>
-    <col min="13" max="13" width="11.17578125" customWidth="true"/>
-    <col min="14" max="14" width="20.90625" customWidth="true"/>
-    <col min="15" max="15" width="10.98828125" customWidth="true"/>
-    <col min="16" max="16" width="10.1328125" customWidth="true"/>
-    <col min="17" max="17" width="39.6328125" customWidth="true"/>
-    <col min="18" max="18" width="11.41015625" customWidth="true"/>
-    <col min="19" max="19" width="13.03515625" customWidth="true"/>
-    <col min="20" max="20" width="11.62109375" customWidth="true"/>
-    <col min="21" max="21" width="8.46875" customWidth="true"/>
-    <col min="22" max="22" width="8.46875" customWidth="true"/>
-    <col min="23" max="23" width="8.46875" customWidth="true"/>
-    <col min="24" max="24" width="7.75" customWidth="true"/>
-    <col min="25" max="25" width="8.83203125" customWidth="true"/>
+    <col min="1" max="1" width="51.609375" customWidth="true"/>
+    <col min="2" max="2" width="6.8828125" customWidth="true"/>
+    <col min="3" max="3" width="24.93359375" customWidth="true"/>
+    <col min="4" max="4" width="43.20703125" customWidth="true"/>
+    <col min="5" max="5" width="33.82421875" customWidth="true"/>
+    <col min="6" max="6" width="8.32421875" customWidth="true"/>
+    <col min="7" max="7" width="7.7890625" customWidth="true"/>
+    <col min="8" max="8" width="7.7890625" customWidth="true"/>
+    <col min="9" max="9" width="26.12890625" customWidth="true"/>
+    <col min="10" max="10" width="42.89453125" customWidth="true"/>
+    <col min="11" max="11" width="42.3671875" customWidth="true"/>
+    <col min="12" max="12" width="17.7578125" customWidth="true"/>
+    <col min="13" max="13" width="11.42578125" customWidth="true"/>
+    <col min="14" max="14" width="21.453125" customWidth="true"/>
+    <col min="15" max="15" width="11.6015625" customWidth="true"/>
+    <col min="16" max="16" width="10.38671875" customWidth="true"/>
+    <col min="17" max="17" width="40.93359375" customWidth="true"/>
+    <col min="18" max="18" width="11.55859375" customWidth="true"/>
+    <col min="19" max="19" width="13.30859375" customWidth="true"/>
+    <col min="20" max="20" width="11.70703125" customWidth="true"/>
+    <col min="21" max="21" width="8.57421875" customWidth="true"/>
+    <col min="22" max="22" width="8.57421875" customWidth="true"/>
+    <col min="23" max="23" width="8.57421875" customWidth="true"/>
+    <col min="24" max="24" width="7.953125" customWidth="true"/>
+    <col min="25" max="25" width="9.20703125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>00162 - 1080p bandwidth - V1.0 - 2022/12/05 - 15:08:40</t>
+          <t>00085 - digital interface - V1.0 - 2023/06/20 - 11:27:54</t>
         </is>
       </c>
     </row>

</xml_diff>